<commit_message>
En proceso de documentación versión 5.
</commit_message>
<xml_diff>
--- a/tb_processes77.xlsx
+++ b/tb_processes77.xlsx
@@ -19,83 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
-  <si>
-    <t>"1-2"</t>
-  </si>
-  <si>
-    <t>"2-3"</t>
-  </si>
-  <si>
-    <t>"3-4</t>
-  </si>
-  <si>
-    <t>"4-5"</t>
-  </si>
-  <si>
-    <t>"5-6"</t>
-  </si>
-  <si>
-    <t>"6-7"</t>
-  </si>
-  <si>
-    <t>"7-8"</t>
-  </si>
-  <si>
-    <t>"8-9"</t>
-  </si>
-  <si>
-    <t>"9-10"</t>
-  </si>
-  <si>
-    <t>"10-11"</t>
-  </si>
-  <si>
-    <t>"11-12"</t>
-  </si>
-  <si>
-    <t>"12-13"</t>
-  </si>
-  <si>
-    <t>"13-14"</t>
-  </si>
-  <si>
-    <t>"14-15"</t>
-  </si>
-  <si>
-    <t>"15-16"</t>
-  </si>
-  <si>
-    <t>"16-17"</t>
-  </si>
-  <si>
-    <t>"17-18"</t>
-  </si>
-  <si>
-    <t>"18-19"</t>
-  </si>
-  <si>
-    <t>"19-20"</t>
-  </si>
-  <si>
-    <t>"isothermal"</t>
-  </si>
-  <si>
-    <t>"adiabatic"</t>
-  </si>
-  <si>
-    <t>"isobaric"</t>
-  </si>
-  <si>
-    <t>"isochoric"</t>
-  </si>
-  <si>
-    <t>"initial_final_states"</t>
-  </si>
-  <si>
-    <t>"type_of_process"</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,172 +339,216 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
+      <c r="A1" t="str">
+        <f>"initial_final_states"</f>
+        <v>initial_final_states</v>
+      </c>
+      <c r="B1" t="str">
+        <f>"type_of_process"</f>
+        <v>type_of_process</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
+      <c r="A2" s="1" t="str">
+        <f>"1-2"</f>
+        <v>1-2</v>
+      </c>
+      <c r="B2" t="str">
+        <f>"isothermal"</f>
+        <v>isothermal</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+      <c r="A3" s="1" t="str">
+        <f>"2-3"</f>
+        <v>2-3</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"adiabatic"</f>
+        <v>adiabatic</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
+      <c r="A4" t="str">
+        <f>"3-4"</f>
+        <v>3-4</v>
+      </c>
+      <c r="B4" t="str">
+        <f>"adiabatic"</f>
+        <v>adiabatic</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
+      <c r="A5" t="str">
+        <f>"4-5"</f>
+        <v>4-5</v>
+      </c>
+      <c r="B5" t="str">
+        <f>"isobaric"</f>
+        <v>isobaric</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
+      <c r="A6" t="str">
+        <f>"5-6"</f>
+        <v>5-6</v>
+      </c>
+      <c r="B6" t="str">
+        <f>"isothermal"</f>
+        <v>isothermal</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
+      <c r="A7" t="str">
+        <f>"6-7"</f>
+        <v>6-7</v>
+      </c>
+      <c r="B7" t="str">
+        <f>"isochoric"</f>
+        <v>isochoric</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
+      <c r="A8" t="str">
+        <f>"7-8"</f>
+        <v>7-8</v>
+      </c>
+      <c r="B8" t="str">
+        <f>"adiabatic"</f>
+        <v>adiabatic</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
+      <c r="A9" t="str">
+        <f>"8-9"</f>
+        <v>8-9</v>
+      </c>
+      <c r="B9" t="str">
+        <f>"isochoric"</f>
+        <v>isochoric</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
+      <c r="A10" t="str">
+        <f>"9-10"</f>
+        <v>9-10</v>
+      </c>
+      <c r="B10" t="str">
+        <f>"isobaric"</f>
+        <v>isobaric</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
+      <c r="A11" t="str">
+        <f>"10-11"</f>
+        <v>10-11</v>
+      </c>
+      <c r="B11" t="str">
+        <f>"isobaric"</f>
+        <v>isobaric</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
+      <c r="A12" t="str">
+        <f>"11-12"</f>
+        <v>11-12</v>
+      </c>
+      <c r="B12" t="str">
+        <f>"isothermal"</f>
+        <v>isothermal</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
+      <c r="A13" t="str">
+        <f>"12-13"</f>
+        <v>12-13</v>
+      </c>
+      <c r="B13" t="str">
+        <f>"isochoric"</f>
+        <v>isochoric</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
+      <c r="A14" t="str">
+        <f>"13-14"</f>
+        <v>13-14</v>
+      </c>
+      <c r="B14" t="str">
+        <f>"adiabatic"</f>
+        <v>adiabatic</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
+      <c r="A15" t="str">
+        <f>"14-15"</f>
+        <v>14-15</v>
+      </c>
+      <c r="B15" t="str">
+        <f>"isochoric"</f>
+        <v>isochoric</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
+      <c r="A16" t="str">
+        <f>"15-16"</f>
+        <v>15-16</v>
+      </c>
+      <c r="B16" t="str">
+        <f>"isochoric"</f>
+        <v>isochoric</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
+      <c r="A17" t="str">
+        <f>"16-17"</f>
+        <v>16-17</v>
+      </c>
+      <c r="B17" t="str">
+        <f>"adiabatic"</f>
+        <v>adiabatic</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
+      <c r="A18" t="str">
+        <f>"17-18"</f>
+        <v>17-18</v>
+      </c>
+      <c r="B18" t="str">
+        <f>"isothermal"</f>
+        <v>isothermal</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
+      <c r="A19" t="str">
+        <f>"18-19"</f>
+        <v>18-19</v>
+      </c>
+      <c r="B19" t="str">
+        <f>"isobaric"</f>
+        <v>isobaric</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
+      <c r="A20" t="str">
+        <f>"19-20"</f>
+        <v>19-20</v>
+      </c>
+      <c r="B20" t="str">
+        <f>"isobaric"</f>
+        <v>isobaric</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8 B14" formula="1"/>
+    <ignoredError sqref="A13" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>